<commit_message>
Auto-committed on 2021/12/03 週五
Former-commit-id: 22d0e96d650f5963e8e7f238b805cfe445326f5e
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L7-介接外部系統/Ias39Loss.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L7-介接外部系統/Ias39Loss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\DB\GenTables\L7-介接外部系統\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A281E7-DE34-4F7E-AAEC-9B67094EBF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAA7804-6F6A-47FD-97E3-24D24A7313C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,7 +961,7 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1198,7 @@
         <v>42</v>
       </c>
       <c r="E14" s="27">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="25" t="s">

</xml_diff>